<commit_message>
Added support for TC without steps
</commit_message>
<xml_diff>
--- a/TC_List.xlsx
+++ b/TC_List.xlsx
@@ -24,7 +24,7 @@
     <t>Key</t>
   </si>
   <si>
-    <t>TC-138690</t>
+    <t>TC-137029</t>
   </si>
 </sst>
 </file>
@@ -345,7 +345,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added HTML description to Jira markup error protection
</commit_message>
<xml_diff>
--- a/TC_List.xlsx
+++ b/TC_List.xlsx
@@ -24,7 +24,7 @@
     <t>Key</t>
   </si>
   <si>
-    <t>TC-137029</t>
+    <t>TC-93055</t>
   </si>
 </sst>
 </file>
@@ -345,7 +345,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changed a log message
</commit_message>
<xml_diff>
--- a/TC_List.xlsx
+++ b/TC_List.xlsx
@@ -24,7 +24,7 @@
     <t>Key</t>
   </si>
   <si>
-    <t>TC-28433</t>
+    <t>TC-131914</t>
   </si>
 </sst>
 </file>
@@ -345,7 +345,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changed log output file name
</commit_message>
<xml_diff>
--- a/TC_List.xlsx
+++ b/TC_List.xlsx
@@ -24,7 +24,7 @@
     <t>Key</t>
   </si>
   <si>
-    <t>TC-131914</t>
+    <t>TC-108251</t>
   </si>
 </sst>
 </file>
@@ -345,7 +345,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>